<commit_message>
Fin du developpement reste doc à faire
</commit_message>
<xml_diff>
--- a/doc/planning_prévisionnel.xlsx
+++ b/doc/planning_prévisionnel.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11880"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15720" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$B$3:$V$23</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Feuil1!$B$3:$V$27</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Jour</t>
   </si>
@@ -90,13 +90,25 @@
   </si>
   <si>
     <t>Historisation des prix</t>
+  </si>
+  <si>
+    <t>PRODUITS</t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>Affichage des produits en fonction de la catégorie</t>
+  </si>
+  <si>
+    <t>Filtres</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +119,20 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -413,7 +439,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -426,8 +452,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -436,44 +460,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -483,8 +474,55 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,10 +803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V24"/>
+  <dimension ref="B2:V28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:V23"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,62 +816,62 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
     </row>
     <row r="3" spans="2:22" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="32">
+      <c r="C3" s="17">
         <v>1</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="30">
+      <c r="D3" s="17"/>
+      <c r="E3" s="15">
         <v>2</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="G3" s="32">
+      <c r="F3" s="15"/>
+      <c r="G3" s="17">
         <v>3</v>
       </c>
-      <c r="H3" s="32"/>
-      <c r="I3" s="30">
+      <c r="H3" s="17"/>
+      <c r="I3" s="15">
         <v>4</v>
       </c>
-      <c r="J3" s="30"/>
-      <c r="K3" s="32">
+      <c r="J3" s="15"/>
+      <c r="K3" s="17">
         <v>5</v>
       </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="30">
+      <c r="L3" s="17"/>
+      <c r="M3" s="15">
         <v>6</v>
       </c>
-      <c r="N3" s="30"/>
-      <c r="O3" s="32">
+      <c r="N3" s="15"/>
+      <c r="O3" s="17">
         <v>7</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="30">
+      <c r="P3" s="17"/>
+      <c r="Q3" s="15">
         <v>8</v>
       </c>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30">
+      <c r="R3" s="15"/>
+      <c r="S3" s="15">
         <v>9</v>
       </c>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30">
+      <c r="T3" s="15"/>
+      <c r="U3" s="15">
         <v>10</v>
       </c>
-      <c r="V3" s="30"/>
-    </row>
-    <row r="4" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="V3" s="15"/>
+    </row>
+    <row r="4" spans="2:22" ht="21.75" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="18" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>2</v>
       </c>
       <c r="E4" s="1">
@@ -891,12 +929,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="13" t="s">
+    <row r="5" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="9"/>
+      <c r="D5" s="7"/>
       <c r="E5" s="4"/>
       <c r="F5" s="5"/>
       <c r="G5" s="4"/>
@@ -917,11 +955,11 @@
       <c r="V5" s="5"/>
     </row>
     <row r="6" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="9"/>
+      <c r="D6" s="7"/>
       <c r="E6" s="4"/>
       <c r="F6" s="5"/>
       <c r="G6" s="4"/>
@@ -941,12 +979,12 @@
       <c r="U6" s="4"/>
       <c r="V6" s="5"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="9"/>
+      <c r="D7" s="7"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
       <c r="G7" s="4"/>
@@ -966,12 +1004,12 @@
       <c r="U7" s="4"/>
       <c r="V7" s="5"/>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
+    <row r="8" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="25" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="7"/>
       <c r="E8" s="4"/>
       <c r="F8" s="5"/>
       <c r="G8" s="4"/>
@@ -992,11 +1030,11 @@
       <c r="V8" s="5"/>
     </row>
     <row r="9" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="7"/>
       <c r="E9" s="4"/>
       <c r="F9" s="5"/>
       <c r="G9" s="4"/>
@@ -1016,12 +1054,12 @@
       <c r="U9" s="4"/>
       <c r="V9" s="5"/>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+    <row r="10" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="24" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="10"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -1041,12 +1079,12 @@
       <c r="U10" s="4"/>
       <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+    <row r="11" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="10"/>
+      <c r="D11" s="8"/>
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
@@ -1066,12 +1104,12 @@
       <c r="U11" s="4"/>
       <c r="V11" s="5"/>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+    <row r="12" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="10"/>
+      <c r="D12" s="8"/>
       <c r="E12" s="4"/>
       <c r="F12" s="5"/>
       <c r="G12" s="4"/>
@@ -1092,11 +1130,11 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="22" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="10"/>
+      <c r="D13" s="8"/>
       <c r="E13" s="4"/>
       <c r="F13" s="5"/>
       <c r="G13" s="4"/>
@@ -1116,34 +1154,34 @@
       <c r="U13" s="4"/>
       <c r="V13" s="5"/>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B14" s="22" t="s">
+    <row r="14" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="18"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="18"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="18"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="18"/>
-      <c r="S14" s="16"/>
-      <c r="T14" s="18"/>
-      <c r="U14" s="16"/>
-      <c r="V14" s="18"/>
-    </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="22" t="s">
-        <v>20</v>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="10"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="10"/>
+      <c r="V14" s="12"/>
+    </row>
+    <row r="15" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
+        <v>12</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
@@ -1161,14 +1199,14 @@
       <c r="P15" s="5"/>
       <c r="Q15" s="4"/>
       <c r="R15" s="5"/>
-      <c r="S15" s="21"/>
+      <c r="S15" s="13"/>
       <c r="T15" s="5"/>
       <c r="U15" s="4"/>
       <c r="V15" s="5"/>
     </row>
-    <row r="16" spans="2:22" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
-        <v>12</v>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B16" s="27" t="s">
+        <v>20</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
@@ -1186,13 +1224,13 @@
       <c r="P16" s="5"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="5"/>
-      <c r="S16" s="21"/>
+      <c r="S16" s="13"/>
       <c r="T16" s="5"/>
       <c r="U16" s="4"/>
       <c r="V16" s="5"/>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="28" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="4"/>
@@ -1211,14 +1249,14 @@
       <c r="P17" s="5"/>
       <c r="Q17" s="4"/>
       <c r="R17" s="5"/>
-      <c r="S17" s="21"/>
+      <c r="S17" s="13"/>
       <c r="T17" s="5"/>
       <c r="U17" s="4"/>
       <c r="V17" s="5"/>
     </row>
     <row r="18" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="25" t="s">
-        <v>14</v>
+      <c r="B18" s="21" t="s">
+        <v>21</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -1236,14 +1274,14 @@
       <c r="P18" s="5"/>
       <c r="Q18" s="4"/>
       <c r="R18" s="5"/>
-      <c r="S18" s="21"/>
+      <c r="S18" s="13"/>
       <c r="T18" s="5"/>
       <c r="U18" s="4"/>
       <c r="V18" s="5"/>
     </row>
-    <row r="19" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
-        <v>15</v>
+    <row r="19" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B19" s="28" t="s">
+        <v>22</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
@@ -1261,14 +1299,14 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="4"/>
       <c r="R19" s="5"/>
-      <c r="S19" s="21"/>
+      <c r="S19" s="13"/>
       <c r="T19" s="5"/>
       <c r="U19" s="4"/>
       <c r="V19" s="5"/>
     </row>
     <row r="20" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="27" t="s">
-        <v>16</v>
+      <c r="B20" s="28" t="s">
+        <v>24</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
@@ -1286,14 +1324,14 @@
       <c r="P20" s="5"/>
       <c r="Q20" s="4"/>
       <c r="R20" s="5"/>
-      <c r="S20" s="21"/>
+      <c r="S20" s="13"/>
       <c r="T20" s="5"/>
       <c r="U20" s="4"/>
       <c r="V20" s="5"/>
     </row>
-    <row r="21" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="27" t="s">
-        <v>17</v>
+    <row r="21" spans="2:22" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="B21" s="26" t="s">
+        <v>23</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
@@ -1311,62 +1349,162 @@
       <c r="P21" s="5"/>
       <c r="Q21" s="4"/>
       <c r="R21" s="5"/>
-      <c r="S21" s="21"/>
+      <c r="S21" s="13"/>
       <c r="T21" s="5"/>
       <c r="U21" s="4"/>
       <c r="V21" s="5"/>
     </row>
-    <row r="22" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="22" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="5"/>
+    </row>
+    <row r="23" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="5"/>
+      <c r="S23" s="13"/>
+      <c r="T23" s="5"/>
+      <c r="U23" s="4"/>
+      <c r="V23" s="5"/>
+    </row>
+    <row r="24" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="5"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="5"/>
+      <c r="U24" s="4"/>
+      <c r="V24" s="5"/>
+    </row>
+    <row r="25" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="36"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="37"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="37"/>
+      <c r="M25" s="36"/>
+      <c r="N25" s="37"/>
+      <c r="O25" s="36"/>
+      <c r="P25" s="37"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="37"/>
+      <c r="S25" s="38"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="36"/>
+      <c r="V25" s="37"/>
+    </row>
+    <row r="26" spans="2:22" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B26" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="18"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="16"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="18"/>
-      <c r="O22" s="16"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="18"/>
-      <c r="U22" s="16"/>
-      <c r="V22" s="18"/>
-    </row>
-    <row r="23" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="29" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="10"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="10"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="14"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="10"/>
+      <c r="V26" s="12"/>
+    </row>
+    <row r="27" spans="2:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="6"/>
-      <c r="D23" s="34"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="7"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="7"/>
-      <c r="O23" s="6"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="6"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="7"/>
-    </row>
-    <row r="24" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="33"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="33"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="33"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="33"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="33"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="33"/>
+      <c r="V27" s="35"/>
+    </row>
+    <row r="28" spans="2:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="Q3:R3"/>

</xml_diff>